<commit_message>
just get this over with bruh
</commit_message>
<xml_diff>
--- a/UMS_Data.xlsx
+++ b/UMS_Data.xlsx
@@ -2,6 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Subjects" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Courses" sheetId="2" r:id="rId5"/>
@@ -9,7 +12,6 @@
     <sheet state="visible" name="Faculties " sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Events " sheetId="5" r:id="rId8"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="185">
   <si>
     <t>Subject Code</t>
   </si>
@@ -569,6 +571,12 @@
   </si>
   <si>
     <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
+  </si>
+  <si>
+    <t>121 Maple St.</t>
+  </si>
+  <si>
+    <t>555-1235</t>
   </si>
 </sst>
 </file>
@@ -902,14 +910,15 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.0"/>
-    <col customWidth="1" min="2" max="2" width="25.63"/>
-    <col customWidth="1" min="3" max="26" width="18.0"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="2" max="2" customWidth="true" width="25.63"/>
+    <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -4965,21 +4974,22 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.25"/>
-    <col customWidth="1" min="2" max="2" width="27.0"/>
-    <col customWidth="1" min="3" max="3" width="12.75"/>
-    <col customWidth="1" min="4" max="4" width="15.38"/>
-    <col customWidth="1" min="5" max="5" width="8.75"/>
-    <col customWidth="1" min="6" max="6" width="16.88"/>
-    <col customWidth="1" min="7" max="7" width="20.63"/>
-    <col customWidth="1" min="8" max="8" width="9.63"/>
-    <col customWidth="1" min="9" max="9" width="16.63"/>
-    <col customWidth="1" min="10" max="26" width="10.88"/>
+    <col min="1" max="1" customWidth="true" width="12.25"/>
+    <col min="2" max="2" customWidth="true" width="27.0"/>
+    <col min="3" max="3" customWidth="true" width="12.75"/>
+    <col min="4" max="4" customWidth="true" width="15.38"/>
+    <col min="5" max="5" customWidth="true" width="8.75"/>
+    <col min="6" max="6" customWidth="true" width="16.88"/>
+    <col min="7" max="7" customWidth="true" width="20.63"/>
+    <col min="8" max="8" customWidth="true" width="9.63"/>
+    <col min="9" max="9" customWidth="true" width="16.63"/>
+    <col min="10" max="26" customWidth="true" width="10.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="1">
@@ -6303,23 +6313,24 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.0"/>
-    <col customWidth="1" min="2" max="2" width="14.13"/>
-    <col customWidth="1" min="3" max="3" width="12.38"/>
-    <col customWidth="1" min="4" max="4" width="10.13"/>
-    <col customWidth="1" min="5" max="5" width="18.88"/>
-    <col customWidth="1" min="6" max="6" width="14.63"/>
-    <col customWidth="1" min="7" max="7" width="16.0"/>
-    <col customWidth="1" min="8" max="8" width="12.25"/>
-    <col customWidth="1" min="9" max="9" width="26.88"/>
-    <col customWidth="1" min="10" max="10" width="72.13"/>
-    <col customWidth="1" min="11" max="11" width="8.75"/>
-    <col customWidth="1" min="12" max="26" width="10.0"/>
+    <col min="1" max="1" customWidth="true" width="10.0"/>
+    <col min="2" max="2" customWidth="true" width="14.13"/>
+    <col min="3" max="3" customWidth="true" width="12.38"/>
+    <col min="4" max="4" customWidth="true" width="10.13"/>
+    <col min="5" max="5" customWidth="true" width="18.88"/>
+    <col min="6" max="6" customWidth="true" width="14.63"/>
+    <col min="7" max="7" customWidth="true" width="16.0"/>
+    <col min="8" max="8" customWidth="true" width="12.25"/>
+    <col min="9" max="9" customWidth="true" width="26.88"/>
+    <col min="10" max="10" customWidth="true" width="72.13"/>
+    <col min="11" max="11" customWidth="true" width="8.75"/>
+    <col min="12" max="26" customWidth="true" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1">
@@ -7745,20 +7756,21 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.63"/>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="8.38"/>
-    <col customWidth="1" min="4" max="4" width="22.38"/>
-    <col customWidth="1" min="5" max="5" width="21.75"/>
-    <col customWidth="1" min="6" max="6" width="14.25"/>
-    <col customWidth="1" min="7" max="7" width="20.0"/>
-    <col customWidth="1" min="8" max="8" width="9.38"/>
-    <col customWidth="1" min="9" max="26" width="8.63"/>
+    <col min="1" max="1" customWidth="true" width="11.63"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="8.38"/>
+    <col min="4" max="4" customWidth="true" width="22.38"/>
+    <col min="5" max="5" customWidth="true" width="21.75"/>
+    <col min="6" max="6" customWidth="true" width="14.25"/>
+    <col min="7" max="7" customWidth="true" width="20.0"/>
+    <col min="8" max="8" customWidth="true" width="9.38"/>
+    <col min="9" max="26" customWidth="true" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8910,21 +8922,22 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.38"/>
-    <col customWidth="1" min="2" max="2" width="18.88"/>
-    <col customWidth="1" min="3" max="3" width="18.63"/>
-    <col customWidth="1" min="4" max="4" width="10.88"/>
-    <col customWidth="1" min="5" max="5" width="14.63"/>
-    <col customWidth="1" min="6" max="6" width="8.63"/>
-    <col customWidth="1" min="7" max="7" width="9.88"/>
-    <col customWidth="1" min="8" max="8" width="13.25"/>
-    <col customWidth="1" min="9" max="9" width="52.25"/>
-    <col customWidth="1" min="10" max="26" width="8.63"/>
+    <col min="1" max="1" customWidth="true" width="10.38"/>
+    <col min="2" max="2" customWidth="true" width="18.88"/>
+    <col min="3" max="3" customWidth="true" width="18.63"/>
+    <col min="4" max="4" customWidth="true" width="10.88"/>
+    <col min="5" max="5" customWidth="true" width="14.63"/>
+    <col min="6" max="6" customWidth="true" width="8.63"/>
+    <col min="7" max="7" customWidth="true" width="9.88"/>
+    <col min="8" max="8" customWidth="true" width="13.25"/>
+    <col min="9" max="9" customWidth="true" width="52.25"/>
+    <col min="10" max="26" customWidth="true" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>